<commit_message>
Graph value adjusted for better result
</commit_message>
<xml_diff>
--- a/Speech Recognition.xlsx
+++ b/Speech Recognition.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tutorial Stuffs\Python Stuffs\Python Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Tutorial Stuffs\Python Stuffs\Python Projects\optimizedSTT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E757B152-1560-4E21-91E5-D54C317AEC79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E88A0-4F4C-467B-A17F-4D3A010D610D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{9ED2CF56-0BD5-4CA8-8E98-77771F1E2FB7}"/>
   </bookViews>
@@ -157,8 +157,260 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0962-4F29-A23B-2D704A7B5205}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="28575">
               <a:solidFill>
@@ -456,7 +708,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9505-437E-8E9B-110B3C4D0075}"/>
+              <c16:uniqueId val="{00000004-0962-4F29-A23B-2D704A7B5205}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -734,14 +986,716 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="43000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Speech Recognition</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="70" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="20000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.9989258605421155E-3"/>
+                  <c:y val="7.2506390649931626E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$38:$C$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1900</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2100</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2400</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2700</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2900</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$38:$D$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.93</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.89</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.85</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.55</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0962-4F29-A23B-2D704A7B5205}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2022268303"/>
+        <c:axId val="2072455327"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2022268303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy Threshold</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2072455327"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2072455327"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Dynamic Energy Ratio</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="50000"/>
+                    <a:lumOff val="50000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2022268303"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
   </c:chart>
   <c:spPr>
     <a:gradFill flip="none" rotWithShape="1">
@@ -829,7 +1783,567 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="43000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="20000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="0" kern="1200" spc="70" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="63500" cap="rnd" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="244">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1382,6 +2896,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>273327</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>162339</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>8697</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>129001</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63B75F5E-0313-41DF-A6E5-E688BBD10C5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1687,10 +3237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3C1322D-C8BF-4374-A7EC-F3F48D38088C}">
-  <dimension ref="C2:E34"/>
+  <dimension ref="C2:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T59" sqref="T59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,6 +3641,414 @@
         <v>4500</v>
       </c>
     </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>34</v>
+      </c>
+      <c r="E38">
+        <f>C38*D38</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>20</v>
+      </c>
+      <c r="D39">
+        <v>17</v>
+      </c>
+      <c r="E39">
+        <f>C39*D39</f>
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>30</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40">
+        <f>C40*D40</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>50</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <f>C41*D41</f>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <f t="shared" ref="E42:E71" si="1">C42*D42</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>200</v>
+      </c>
+      <c r="D43">
+        <v>2.5</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>300</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>400</v>
+      </c>
+      <c r="D45">
+        <v>1.93</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>772</v>
+      </c>
+    </row>
+    <row r="46" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>500</v>
+      </c>
+      <c r="D46">
+        <v>1.89</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>945</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>600</v>
+      </c>
+      <c r="D47">
+        <v>1.85</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>700</v>
+      </c>
+      <c r="D48">
+        <v>1.8</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>800</v>
+      </c>
+      <c r="D49">
+        <v>1.76</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>1408</v>
+      </c>
+    </row>
+    <row r="50" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>900</v>
+      </c>
+      <c r="D50">
+        <v>1.72</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="51" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>1000</v>
+      </c>
+      <c r="D51">
+        <v>1.65</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="52" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>1100</v>
+      </c>
+      <c r="D52">
+        <v>1.62</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>1782.0000000000002</v>
+      </c>
+    </row>
+    <row r="53" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>1200</v>
+      </c>
+      <c r="D53">
+        <v>1.6</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="54" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>1300</v>
+      </c>
+      <c r="D54">
+        <v>1.55</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="55" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>1400</v>
+      </c>
+      <c r="D55">
+        <v>1.5</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="56" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>1500</v>
+      </c>
+      <c r="D56">
+        <v>1.5</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="57" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>1600</v>
+      </c>
+      <c r="D57">
+        <v>1.5</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="58" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>1700</v>
+      </c>
+      <c r="D58">
+        <v>1.5</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="59" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>1800</v>
+      </c>
+      <c r="D59">
+        <v>1.5</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="60" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>1900</v>
+      </c>
+      <c r="D60">
+        <v>1.5</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>2850</v>
+      </c>
+    </row>
+    <row r="61" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>2000</v>
+      </c>
+      <c r="D61">
+        <v>1.5</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="62" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>2100</v>
+      </c>
+      <c r="D62">
+        <v>1.5</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="63" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>2200</v>
+      </c>
+      <c r="D63">
+        <v>1.5</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="64" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>2300</v>
+      </c>
+      <c r="D64">
+        <v>1.5</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>2400</v>
+      </c>
+      <c r="D65">
+        <v>1.5</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>2500</v>
+      </c>
+      <c r="D66">
+        <v>1.5</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>2600</v>
+      </c>
+      <c r="D67">
+        <v>1.5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>2700</v>
+      </c>
+      <c r="D68">
+        <v>1.5</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>2800</v>
+      </c>
+      <c r="D69">
+        <v>1.5</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>2900</v>
+      </c>
+      <c r="D70">
+        <v>1.5</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>4350</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>3000</v>
+      </c>
+      <c r="D71">
+        <v>1.5</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>